<commit_message>
final files for SPE Hackaton 2020
</commit_message>
<xml_diff>
--- a/archivo_descargado2018.xlsx
+++ b/archivo_descargado2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\misdocumentos\sperfiles\liliana.boton\Desktop\REPORTE MENSUAL PRODUCCIÓN\DANE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\germa\Documents\Python exercices\spe-hackaton\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547D6BAC-7600-4B11-AA25-4FB4AEA4591B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crudo Fiscalizado Bpdc" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Crudo Fiscalizado Bpdc'!$A$3:$Q$473</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2165,7 +2175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2664,23 +2674,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q477"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.265625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.59765625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.3984375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="73.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2701,7 +2712,7 @@
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2720,7 +2731,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2773,7 +2784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2826,7 +2837,7 @@
         <v>1373.8767741935483</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2879,7 +2890,7 @@
         <v>206.71032258064517</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2932,7 +2943,7 @@
         <v>704.88516129032257</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2985,7 +2996,7 @@
         <v>225.90258064516127</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -3038,7 +3049,7 @@
         <v>10601.76129032258</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -3091,7 +3102,7 @@
         <v>1942.4935483870968</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -3144,7 +3155,7 @@
         <v>1095.5635483870967</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -3197,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -3250,7 +3261,7 @@
         <v>7919.4516129032254</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
@@ -3303,7 +3314,7 @@
         <v>134.38709677419354</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -3356,7 +3367,7 @@
         <v>259.48387096774195</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
@@ -3409,7 +3420,7 @@
         <v>40.12903225806452</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -3462,7 +3473,7 @@
         <v>20978.354838709678</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -3515,7 +3526,7 @@
         <v>3411.0967741935483</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -3568,7 +3579,7 @@
         <v>27.387096774193548</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -3621,7 +3632,7 @@
         <v>192.7741935483871</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
@@ -3674,7 +3685,7 @@
         <v>384.16129032258067</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -3727,7 +3738,7 @@
         <v>137.67741935483872</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
@@ -3780,7 +3791,7 @@
         <v>80.645161290322577</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -3833,7 +3844,7 @@
         <v>1260.0967741935483</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
@@ -3886,7 +3897,7 @@
         <v>1565.8709677419354</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3939,7 +3950,7 @@
         <v>65.870967741935488</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
@@ -3992,7 +4003,7 @@
         <v>148.48387096774192</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
@@ -4045,7 +4056,7 @@
         <v>123.7741935483871</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>37</v>
       </c>
@@ -4098,7 +4109,7 @@
         <v>2707.9354838709678</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
@@ -4151,7 +4162,7 @@
         <v>791.16129032258061</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
@@ -4204,7 +4215,7 @@
         <v>38.064516129032256</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
@@ -4257,7 +4268,7 @@
         <v>991.51612903225805</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>37</v>
       </c>
@@ -4310,7 +4321,7 @@
         <v>17.483870967741936</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
@@ -4363,7 +4374,7 @@
         <v>3175.9354838709678</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>37</v>
       </c>
@@ -4416,7 +4427,7 @@
         <v>4130</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
@@ -4469,7 +4480,7 @@
         <v>7.3029032258064515</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -4522,7 +4533,7 @@
         <v>310.83322580645159</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
@@ -4575,7 +4586,7 @@
         <v>554.34193548387088</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>69</v>
       </c>
@@ -4628,7 +4639,7 @@
         <v>420.30322580645162</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="4" t="s">
         <v>69</v>
       </c>
@@ -4681,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
@@ -4734,7 +4745,7 @@
         <v>11699.51419354839</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
@@ -4787,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
@@ -4840,7 +4851,7 @@
         <v>416.80806451612904</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="4" t="s">
         <v>75</v>
       </c>
@@ -4893,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
@@ -4946,7 +4957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>75</v>
       </c>
@@ -4999,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
         <v>75</v>
       </c>
@@ -5052,7 +5063,7 @@
         <v>17.98</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>75</v>
       </c>
@@ -5105,7 +5116,7 @@
         <v>217.54419354838709</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
         <v>84</v>
       </c>
@@ -5158,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
         <v>84</v>
       </c>
@@ -5211,7 +5222,7 @@
         <v>340.61290322580646</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>84</v>
       </c>
@@ -5264,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A51" s="4" t="s">
         <v>84</v>
       </c>
@@ -5317,7 +5328,7 @@
         <v>763.57032258064521</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" s="4" t="s">
         <v>84</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>6506.9729032258065</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>84</v>
       </c>
@@ -5423,7 +5434,7 @@
         <v>3028.2845161290325</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
         <v>84</v>
       </c>
@@ -5476,7 +5487,7 @@
         <v>3522.1729032258063</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A55" s="4" t="s">
         <v>84</v>
       </c>
@@ -5529,7 +5540,7 @@
         <v>2989.8464516129034</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>84</v>
       </c>
@@ -5582,7 +5593,7 @@
         <v>3917.9306451612906</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
         <v>84</v>
       </c>
@@ -5635,7 +5646,7 @@
         <v>11061.563548387096</v>
       </c>
     </row>
-    <row r="58" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
         <v>84</v>
       </c>
@@ -5688,7 +5699,7 @@
         <v>1137.8145161290322</v>
       </c>
     </row>
-    <row r="59" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>84</v>
       </c>
@@ -5741,7 +5752,7 @@
         <v>59.140322580645162</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A60" s="4" t="s">
         <v>84</v>
       </c>
@@ -5794,7 +5805,7 @@
         <v>41.660322580645165</v>
       </c>
     </row>
-    <row r="61" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A61" s="4" t="s">
         <v>106</v>
       </c>
@@ -5847,7 +5858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>110</v>
       </c>
@@ -5900,7 +5911,7 @@
         <v>1955.4096774193547</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
         <v>110</v>
       </c>
@@ -5953,7 +5964,7 @@
         <v>1081.1825806451614</v>
       </c>
     </row>
-    <row r="64" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A64" s="4" t="s">
         <v>110</v>
       </c>
@@ -6006,7 +6017,7 @@
         <v>5870.8925806451616</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>110</v>
       </c>
@@ -6059,7 +6070,7 @@
         <v>1689.5687096774195</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
         <v>110</v>
       </c>
@@ -6112,7 +6123,7 @@
         <v>3448.2177419354839</v>
       </c>
     </row>
-    <row r="67" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
         <v>110</v>
       </c>
@@ -6165,7 +6176,7 @@
         <v>665.29838709677415</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
         <v>110</v>
       </c>
@@ -6218,7 +6229,7 @@
         <v>415.44935483870967</v>
       </c>
     </row>
-    <row r="69" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A69" s="4" t="s">
         <v>110</v>
       </c>
@@ -6271,7 +6282,7 @@
         <v>26.940645161290323</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A70" s="4" t="s">
         <v>110</v>
       </c>
@@ -6324,7 +6335,7 @@
         <v>276.94387096774193</v>
       </c>
     </row>
-    <row r="71" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
         <v>110</v>
       </c>
@@ -6377,7 +6388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A72" s="4" t="s">
         <v>110</v>
       </c>
@@ -6430,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A73" s="4" t="s">
         <v>110</v>
       </c>
@@ -6483,7 +6494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>110</v>
       </c>
@@ -6536,7 +6547,7 @@
         <v>408.57451612903225</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A75" s="4" t="s">
         <v>110</v>
       </c>
@@ -6589,7 +6600,7 @@
         <v>95.375806451612902</v>
       </c>
     </row>
-    <row r="76" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
         <v>110</v>
       </c>
@@ -6642,7 +6653,7 @@
         <v>362.30290322580646</v>
       </c>
     </row>
-    <row r="77" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" s="4" t="s">
         <v>110</v>
       </c>
@@ -6695,7 +6706,7 @@
         <v>816.60387096774195</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A78" s="4" t="s">
         <v>110</v>
       </c>
@@ -6748,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A79" s="4" t="s">
         <v>110</v>
       </c>
@@ -6801,7 +6812,7 @@
         <v>356.54838709677421</v>
       </c>
     </row>
-    <row r="80" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>110</v>
       </c>
@@ -6854,7 +6865,7 @@
         <v>704.05483870967748</v>
       </c>
     </row>
-    <row r="81" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A81" s="4" t="s">
         <v>110</v>
       </c>
@@ -6907,7 +6918,7 @@
         <v>394.39354838709681</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A82" s="4" t="s">
         <v>110</v>
       </c>
@@ -6960,7 +6971,7 @@
         <v>265.8041935483871</v>
       </c>
     </row>
-    <row r="83" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>110</v>
       </c>
@@ -7013,7 +7024,7 @@
         <v>521.90354838709675</v>
       </c>
     </row>
-    <row r="84" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
         <v>110</v>
       </c>
@@ -7066,7 +7077,7 @@
         <v>177.08354838709678</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
         <v>110</v>
       </c>
@@ -7119,7 +7130,7 @@
         <v>81.638709677419357</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>110</v>
       </c>
@@ -7172,7 +7183,7 @@
         <v>47.669032258064519</v>
       </c>
     </row>
-    <row r="87" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" s="4" t="s">
         <v>110</v>
       </c>
@@ -7225,7 +7236,7 @@
         <v>392.54354838709679</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
         <v>110</v>
       </c>
@@ -7278,7 +7289,7 @@
         <v>1062.5735483870967</v>
       </c>
     </row>
-    <row r="89" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" s="4" t="s">
         <v>110</v>
       </c>
@@ -7331,7 +7342,7 @@
         <v>15.784193548387098</v>
       </c>
     </row>
-    <row r="90" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" s="4" t="s">
         <v>110</v>
       </c>
@@ -7384,7 +7395,7 @@
         <v>84.074516129032261</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" s="4" t="s">
         <v>110</v>
       </c>
@@ -7437,7 +7448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>110</v>
       </c>
@@ -7490,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" s="4" t="s">
         <v>110</v>
       </c>
@@ -7543,7 +7554,7 @@
         <v>1101.4225806451611</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" s="4" t="s">
         <v>110</v>
       </c>
@@ -7596,7 +7607,7 @@
         <v>723.81774193548381</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" s="4" t="s">
         <v>110</v>
       </c>
@@ -7649,7 +7660,7 @@
         <v>607.81032258064522</v>
       </c>
     </row>
-    <row r="96" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" s="4" t="s">
         <v>110</v>
       </c>
@@ -7702,7 +7713,7 @@
         <v>1616.2412903225804</v>
       </c>
     </row>
-    <row r="97" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>110</v>
       </c>
@@ -7755,7 +7766,7 @@
         <v>148.22387096774193</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>110</v>
       </c>
@@ -7808,7 +7819,7 @@
         <v>283.7483870967742</v>
       </c>
     </row>
-    <row r="99" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" s="4" t="s">
         <v>110</v>
       </c>
@@ -7861,7 +7872,7 @@
         <v>152.22193548387096</v>
       </c>
     </row>
-    <row r="100" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" s="4" t="s">
         <v>110</v>
       </c>
@@ -7914,7 +7925,7 @@
         <v>535.99709677419355</v>
       </c>
     </row>
-    <row r="101" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" s="4" t="s">
         <v>110</v>
       </c>
@@ -7967,7 +7978,7 @@
         <v>72.760000000000005</v>
       </c>
     </row>
-    <row r="102" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" s="4" t="s">
         <v>110</v>
       </c>
@@ -8020,7 +8031,7 @@
         <v>197.9925806451613</v>
       </c>
     </row>
-    <row r="103" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" s="4" t="s">
         <v>110</v>
       </c>
@@ -8073,7 +8084,7 @@
         <v>151.18451612903226</v>
       </c>
     </row>
-    <row r="104" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" s="4" t="s">
         <v>110</v>
       </c>
@@ -8126,7 +8137,7 @@
         <v>70.013548387096776</v>
       </c>
     </row>
-    <row r="105" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" s="4" t="s">
         <v>110</v>
       </c>
@@ -8179,7 +8190,7 @@
         <v>420.72161290322578</v>
       </c>
     </row>
-    <row r="106" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" s="4" t="s">
         <v>110</v>
       </c>
@@ -8232,7 +8243,7 @@
         <v>43.340322580645157</v>
       </c>
     </row>
-    <row r="107" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" s="4" t="s">
         <v>110</v>
       </c>
@@ -8285,7 +8296,7 @@
         <v>195.09</v>
       </c>
     </row>
-    <row r="108" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" s="4" t="s">
         <v>110</v>
       </c>
@@ -8338,7 +8349,7 @@
         <v>1318.3574193548388</v>
       </c>
     </row>
-    <row r="109" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" s="4" t="s">
         <v>110</v>
       </c>
@@ -8391,7 +8402,7 @@
         <v>132.06032258064516</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" s="4" t="s">
         <v>110</v>
       </c>
@@ -8444,7 +8455,7 @@
         <v>3.544193548387097</v>
       </c>
     </row>
-    <row r="111" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" s="4" t="s">
         <v>110</v>
       </c>
@@ -8497,7 +8508,7 @@
         <v>1405.6780645161289</v>
       </c>
     </row>
-    <row r="112" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" s="4" t="s">
         <v>110</v>
       </c>
@@ -8550,7 +8561,7 @@
         <v>219.96290322580646</v>
       </c>
     </row>
-    <row r="113" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" s="4" t="s">
         <v>110</v>
       </c>
@@ -8603,7 +8614,7 @@
         <v>701.2690322580645</v>
       </c>
     </row>
-    <row r="114" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" s="4" t="s">
         <v>110</v>
       </c>
@@ -8656,7 +8667,7 @@
         <v>72.604838709677423</v>
       </c>
     </row>
-    <row r="115" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" s="4" t="s">
         <v>110</v>
       </c>
@@ -8709,7 +8720,7 @@
         <v>21.502580645161292</v>
       </c>
     </row>
-    <row r="116" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" s="4" t="s">
         <v>110</v>
       </c>
@@ -8762,7 +8773,7 @@
         <v>239.68258064516129</v>
       </c>
     </row>
-    <row r="117" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" s="4" t="s">
         <v>110</v>
       </c>
@@ -8815,7 +8826,7 @@
         <v>46.01064516129032</v>
       </c>
     </row>
-    <row r="118" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" s="4" t="s">
         <v>110</v>
       </c>
@@ -8868,7 +8879,7 @@
         <v>510.00032258064516</v>
       </c>
     </row>
-    <row r="119" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" s="4" t="s">
         <v>110</v>
       </c>
@@ -8921,7 +8932,7 @@
         <v>163.26967741935482</v>
       </c>
     </row>
-    <row r="120" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" s="4" t="s">
         <v>110</v>
       </c>
@@ -8974,7 +8985,7 @@
         <v>59.365806451612897</v>
       </c>
     </row>
-    <row r="121" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" s="4" t="s">
         <v>110</v>
       </c>
@@ -9027,7 +9038,7 @@
         <v>906.45935483870971</v>
       </c>
     </row>
-    <row r="122" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>110</v>
       </c>
@@ -9080,7 +9091,7 @@
         <v>1060.3064516129032</v>
       </c>
     </row>
-    <row r="123" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A123" s="4" t="s">
         <v>110</v>
       </c>
@@ -9133,7 +9144,7 @@
         <v>129.02064516129033</v>
       </c>
     </row>
-    <row r="124" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A124" s="4" t="s">
         <v>110</v>
       </c>
@@ -9186,7 +9197,7 @@
         <v>138.57935483870969</v>
       </c>
     </row>
-    <row r="125" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A125" s="4" t="s">
         <v>110</v>
       </c>
@@ -9239,7 +9250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A126" s="4" t="s">
         <v>110</v>
       </c>
@@ -9292,7 +9303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A127" s="4" t="s">
         <v>110</v>
       </c>
@@ -9345,7 +9356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A128" s="4" t="s">
         <v>110</v>
       </c>
@@ -9398,7 +9409,7 @@
         <v>414.56806451612903</v>
       </c>
     </row>
-    <row r="129" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" s="4" t="s">
         <v>110</v>
       </c>
@@ -9451,7 +9462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A130" s="4" t="s">
         <v>110</v>
       </c>
@@ -9504,7 +9515,7 @@
         <v>49.980645161290326</v>
       </c>
     </row>
-    <row r="131" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A131" s="4" t="s">
         <v>110</v>
       </c>
@@ -9557,7 +9568,7 @@
         <v>90.129032258064512</v>
       </c>
     </row>
-    <row r="132" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A132" s="4" t="s">
         <v>110</v>
       </c>
@@ -9610,7 +9621,7 @@
         <v>121.6774193548387</v>
       </c>
     </row>
-    <row r="133" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A133" s="4" t="s">
         <v>110</v>
       </c>
@@ -9663,7 +9674,7 @@
         <v>483.48580645161286</v>
       </c>
     </row>
-    <row r="134" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A134" s="4" t="s">
         <v>110</v>
       </c>
@@ -9716,7 +9727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A135" s="4" t="s">
         <v>110</v>
       </c>
@@ -9769,7 +9780,7 @@
         <v>161.66096774193548</v>
       </c>
     </row>
-    <row r="136" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A136" s="4" t="s">
         <v>110</v>
       </c>
@@ -9822,7 +9833,7 @@
         <v>852.32935483870961</v>
       </c>
     </row>
-    <row r="137" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A137" s="4" t="s">
         <v>110</v>
       </c>
@@ -9875,7 +9886,7 @@
         <v>1.4887096774193549</v>
       </c>
     </row>
-    <row r="138" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A138" s="4" t="s">
         <v>110</v>
       </c>
@@ -9928,7 +9939,7 @@
         <v>29.198064516129033</v>
       </c>
     </row>
-    <row r="139" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A139" s="4" t="s">
         <v>110</v>
       </c>
@@ -9981,7 +9992,7 @@
         <v>361.45935483870971</v>
       </c>
     </row>
-    <row r="140" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A140" s="4" t="s">
         <v>110</v>
       </c>
@@ -10034,7 +10045,7 @@
         <v>154.24225806451614</v>
       </c>
     </row>
-    <row r="141" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A141" s="4" t="s">
         <v>110</v>
       </c>
@@ -10087,7 +10098,7 @@
         <v>55.168387096774197</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A142" s="4" t="s">
         <v>110</v>
       </c>
@@ -10140,7 +10151,7 @@
         <v>1540.2170967741934</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A143" s="4" t="s">
         <v>110</v>
       </c>
@@ -10193,7 +10204,7 @@
         <v>161.69322580645161</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A144" s="4" t="s">
         <v>110</v>
       </c>
@@ -10246,7 +10257,7 @@
         <v>37.399354838709684</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A145" s="4" t="s">
         <v>110</v>
       </c>
@@ -10299,7 +10310,7 @@
         <v>59.725806451612904</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A146" s="4" t="s">
         <v>110</v>
       </c>
@@ -10352,7 +10363,7 @@
         <v>27.354193548387098</v>
       </c>
     </row>
-    <row r="147" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A147" s="4" t="s">
         <v>110</v>
       </c>
@@ -10405,7 +10416,7 @@
         <v>387.32967741935482</v>
       </c>
     </row>
-    <row r="148" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A148" s="4" t="s">
         <v>110</v>
       </c>
@@ -10458,7 +10469,7 @@
         <v>162.89709677419356</v>
       </c>
     </row>
-    <row r="149" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A149" s="4" t="s">
         <v>110</v>
       </c>
@@ -10511,7 +10522,7 @@
         <v>124.48838709677419</v>
       </c>
     </row>
-    <row r="150" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A150" s="4" t="s">
         <v>110</v>
       </c>
@@ -10564,7 +10575,7 @@
         <v>232.06612903225806</v>
       </c>
     </row>
-    <row r="151" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A151" s="4" t="s">
         <v>110</v>
       </c>
@@ -10617,7 +10628,7 @@
         <v>157.28387096774193</v>
       </c>
     </row>
-    <row r="152" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A152" s="4" t="s">
         <v>110</v>
       </c>
@@ -10670,7 +10681,7 @@
         <v>272.93451612903226</v>
       </c>
     </row>
-    <row r="153" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A153" s="4" t="s">
         <v>110</v>
       </c>
@@ -10723,7 +10734,7 @@
         <v>140.64516129032259</v>
       </c>
     </row>
-    <row r="154" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A154" s="4" t="s">
         <v>110</v>
       </c>
@@ -10776,7 +10787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A155" s="4" t="s">
         <v>110</v>
       </c>
@@ -10829,7 +10840,7 @@
         <v>1228.0148387096774</v>
       </c>
     </row>
-    <row r="156" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A156" s="4" t="s">
         <v>110</v>
       </c>
@@ -10882,7 +10893,7 @@
         <v>164.35290322580644</v>
       </c>
     </row>
-    <row r="157" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A157" s="4" t="s">
         <v>110</v>
       </c>
@@ -10935,7 +10946,7 @@
         <v>74.260967741935488</v>
       </c>
     </row>
-    <row r="158" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A158" s="4" t="s">
         <v>110</v>
       </c>
@@ -10988,7 +10999,7 @@
         <v>76.750322580645175</v>
       </c>
     </row>
-    <row r="159" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A159" s="4" t="s">
         <v>110</v>
       </c>
@@ -11041,7 +11052,7 @@
         <v>149.06741935483871</v>
       </c>
     </row>
-    <row r="160" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A160" s="4" t="s">
         <v>110</v>
       </c>
@@ -11094,7 +11105,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="161" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161" s="4" t="s">
         <v>110</v>
       </c>
@@ -11147,7 +11158,7 @@
         <v>15.103225806451613</v>
       </c>
     </row>
-    <row r="162" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162" s="4" t="s">
         <v>110</v>
       </c>
@@ -11200,7 +11211,7 @@
         <v>134.06903225806454</v>
       </c>
     </row>
-    <row r="163" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A163" s="4" t="s">
         <v>110</v>
       </c>
@@ -11253,7 +11264,7 @@
         <v>61.806451612903224</v>
       </c>
     </row>
-    <row r="164" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A164" s="4" t="s">
         <v>110</v>
       </c>
@@ -11306,7 +11317,7 @@
         <v>196.33483870967743</v>
       </c>
     </row>
-    <row r="165" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A165" s="4" t="s">
         <v>110</v>
       </c>
@@ -11359,7 +11370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A166" s="4" t="s">
         <v>110</v>
       </c>
@@ -11412,7 +11423,7 @@
         <v>2100.3890322580646</v>
       </c>
     </row>
-    <row r="167" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A167" s="4" t="s">
         <v>110</v>
       </c>
@@ -11465,7 +11476,7 @@
         <v>510.00903225806445</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A168" s="4" t="s">
         <v>110</v>
       </c>
@@ -11518,7 +11529,7 @@
         <v>70.976774193548394</v>
       </c>
     </row>
-    <row r="169" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A169" s="4" t="s">
         <v>110</v>
       </c>
@@ -11571,7 +11582,7 @@
         <v>208.51419354838711</v>
       </c>
     </row>
-    <row r="170" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A170" s="4" t="s">
         <v>110</v>
       </c>
@@ -11624,7 +11635,7 @@
         <v>158.68225806451611</v>
       </c>
     </row>
-    <row r="171" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A171" s="4" t="s">
         <v>110</v>
       </c>
@@ -11677,7 +11688,7 @@
         <v>464.09322580645158</v>
       </c>
     </row>
-    <row r="172" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A172" s="4" t="s">
         <v>110</v>
       </c>
@@ -11730,7 +11741,7 @@
         <v>27.166774193548385</v>
       </c>
     </row>
-    <row r="173" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A173" s="4" t="s">
         <v>110</v>
       </c>
@@ -11783,7 +11794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A174" s="4" t="s">
         <v>110</v>
       </c>
@@ -11836,7 +11847,7 @@
         <v>438.5012903225807</v>
       </c>
     </row>
-    <row r="175" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A175" s="4" t="s">
         <v>110</v>
       </c>
@@ -11889,7 +11900,7 @@
         <v>434.21387096774191</v>
       </c>
     </row>
-    <row r="176" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A176" s="4" t="s">
         <v>110</v>
       </c>
@@ -11942,7 +11953,7 @@
         <v>207.4041935483871</v>
       </c>
     </row>
-    <row r="177" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A177" s="4" t="s">
         <v>110</v>
       </c>
@@ -11995,7 +12006,7 @@
         <v>544.56290322580651</v>
       </c>
     </row>
-    <row r="178" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A178" s="4" t="s">
         <v>110</v>
       </c>
@@ -12048,7 +12059,7 @@
         <v>353.21999999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A179" s="4" t="s">
         <v>110</v>
       </c>
@@ -12101,7 +12112,7 @@
         <v>180.81032258064516</v>
       </c>
     </row>
-    <row r="180" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180" s="4" t="s">
         <v>110</v>
       </c>
@@ -12154,7 +12165,7 @@
         <v>245.31322580645161</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181" s="4" t="s">
         <v>110</v>
       </c>
@@ -12207,7 +12218,7 @@
         <v>197.76225806451615</v>
       </c>
     </row>
-    <row r="182" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A182" s="4" t="s">
         <v>110</v>
       </c>
@@ -12260,7 +12271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A183" s="4" t="s">
         <v>110</v>
       </c>
@@ -12313,7 +12324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A184" s="4" t="s">
         <v>110</v>
       </c>
@@ -12366,7 +12377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A185" s="4" t="s">
         <v>110</v>
       </c>
@@ -12419,7 +12430,7 @@
         <v>209.46580645161291</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A186" s="4" t="s">
         <v>110</v>
       </c>
@@ -12472,7 +12483,7 @@
         <v>112.70193548387097</v>
       </c>
     </row>
-    <row r="187" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A187" s="4" t="s">
         <v>110</v>
       </c>
@@ -12525,7 +12536,7 @@
         <v>388.33193548387101</v>
       </c>
     </row>
-    <row r="188" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A188" s="4" t="s">
         <v>110</v>
       </c>
@@ -12578,7 +12589,7 @@
         <v>1358.2470967741936</v>
       </c>
     </row>
-    <row r="189" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A189" s="4" t="s">
         <v>110</v>
       </c>
@@ -12631,7 +12642,7 @@
         <v>1162.0009677419355</v>
       </c>
     </row>
-    <row r="190" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A190" s="4" t="s">
         <v>110</v>
       </c>
@@ -12684,7 +12695,7 @@
         <v>313.56451612903226</v>
       </c>
     </row>
-    <row r="191" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A191" s="4" t="s">
         <v>110</v>
       </c>
@@ -12737,7 +12748,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A192" s="4" t="s">
         <v>110</v>
       </c>
@@ -12790,7 +12801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A193" s="4" t="s">
         <v>110</v>
       </c>
@@ -12843,7 +12854,7 @@
         <v>97.396774193548396</v>
       </c>
     </row>
-    <row r="194" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A194" s="4" t="s">
         <v>110</v>
       </c>
@@ -12896,7 +12907,7 @@
         <v>352.32129032258064</v>
       </c>
     </row>
-    <row r="195" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A195" s="4" t="s">
         <v>110</v>
       </c>
@@ -12949,7 +12960,7 @@
         <v>556.11806451612904</v>
       </c>
     </row>
-    <row r="196" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A196" s="4" t="s">
         <v>110</v>
       </c>
@@ -13002,7 +13013,7 @@
         <v>6421.2767741935486</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A197" s="4" t="s">
         <v>110</v>
       </c>
@@ -13055,7 +13066,7 @@
         <v>16415.950322580647</v>
       </c>
     </row>
-    <row r="198" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" s="4" t="s">
         <v>110</v>
       </c>
@@ -13108,7 +13119,7 @@
         <v>5846.9341935483872</v>
       </c>
     </row>
-    <row r="199" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A199" s="4" t="s">
         <v>110</v>
       </c>
@@ -13161,7 +13172,7 @@
         <v>429.16161290322583</v>
       </c>
     </row>
-    <row r="200" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" s="4" t="s">
         <v>110</v>
       </c>
@@ -13214,7 +13225,7 @@
         <v>4693.4854838709671</v>
       </c>
     </row>
-    <row r="201" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A201" s="4" t="s">
         <v>110</v>
       </c>
@@ -13267,7 +13278,7 @@
         <v>491.08903225806455</v>
       </c>
     </row>
-    <row r="202" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A202" s="4" t="s">
         <v>110</v>
       </c>
@@ -13320,7 +13331,7 @@
         <v>188.45322580645163</v>
       </c>
     </row>
-    <row r="203" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A203" s="4" t="s">
         <v>110</v>
       </c>
@@ -13373,7 +13384,7 @@
         <v>289.7354838709677</v>
       </c>
     </row>
-    <row r="204" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A204" s="4" t="s">
         <v>110</v>
       </c>
@@ -13426,7 +13437,7 @@
         <v>115.12290322580645</v>
       </c>
     </row>
-    <row r="205" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A205" s="4" t="s">
         <v>110</v>
       </c>
@@ -13479,7 +13490,7 @@
         <v>24.491612903225807</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A206" s="4" t="s">
         <v>110</v>
       </c>
@@ -13532,7 +13543,7 @@
         <v>99.251612903225819</v>
       </c>
     </row>
-    <row r="207" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A207" s="4" t="s">
         <v>110</v>
       </c>
@@ -13585,7 +13596,7 @@
         <v>43.943225806451615</v>
       </c>
     </row>
-    <row r="208" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A208" s="4" t="s">
         <v>110</v>
       </c>
@@ -13638,7 +13649,7 @@
         <v>0.55548387096774188</v>
       </c>
     </row>
-    <row r="209" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" s="4" t="s">
         <v>110</v>
       </c>
@@ -13691,7 +13702,7 @@
         <v>668.24548387096775</v>
       </c>
     </row>
-    <row r="210" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" s="4" t="s">
         <v>110</v>
       </c>
@@ -13744,7 +13755,7 @@
         <v>192.5241935483871</v>
       </c>
     </row>
-    <row r="211" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" s="4" t="s">
         <v>110</v>
       </c>
@@ -13797,7 +13808,7 @@
         <v>1888.9125806451614</v>
       </c>
     </row>
-    <row r="212" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" s="4" t="s">
         <v>110</v>
       </c>
@@ -13850,7 +13861,7 @@
         <v>962.68741935483877</v>
       </c>
     </row>
-    <row r="213" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A213" s="4" t="s">
         <v>110</v>
       </c>
@@ -13903,7 +13914,7 @@
         <v>78.088387096774184</v>
       </c>
     </row>
-    <row r="214" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" s="4" t="s">
         <v>110</v>
       </c>
@@ -13956,7 +13967,7 @@
         <v>32.751935483870966</v>
       </c>
     </row>
-    <row r="215" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A215" s="4" t="s">
         <v>110</v>
       </c>
@@ -14009,7 +14020,7 @@
         <v>298.49064516129027</v>
       </c>
     </row>
-    <row r="216" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A216" s="4" t="s">
         <v>110</v>
       </c>
@@ -14062,7 +14073,7 @@
         <v>37.26064516129032</v>
       </c>
     </row>
-    <row r="217" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A217" s="4" t="s">
         <v>110</v>
       </c>
@@ -14115,7 +14126,7 @@
         <v>535.64193548387107</v>
       </c>
     </row>
-    <row r="218" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" s="4" t="s">
         <v>110</v>
       </c>
@@ -14168,7 +14179,7 @@
         <v>314.23032258064512</v>
       </c>
     </row>
-    <row r="219" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" s="4" t="s">
         <v>110</v>
       </c>
@@ -14221,7 +14232,7 @@
         <v>298.2235483870968</v>
       </c>
     </row>
-    <row r="220" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A220" s="4" t="s">
         <v>110</v>
       </c>
@@ -14274,7 +14285,7 @@
         <v>49.272580645161291</v>
       </c>
     </row>
-    <row r="221" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A221" s="4" t="s">
         <v>110</v>
       </c>
@@ -14327,7 +14338,7 @@
         <v>23914.925483870971</v>
       </c>
     </row>
-    <row r="222" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" s="4" t="s">
         <v>110</v>
       </c>
@@ -14380,7 +14391,7 @@
         <v>7146.2529032258062</v>
       </c>
     </row>
-    <row r="223" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A223" s="4" t="s">
         <v>110</v>
       </c>
@@ -14433,7 +14444,7 @@
         <v>1003.7977419354838</v>
       </c>
     </row>
-    <row r="224" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" s="4" t="s">
         <v>110</v>
       </c>
@@ -14486,7 +14497,7 @@
         <v>5725.2412903225813</v>
       </c>
     </row>
-    <row r="225" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A225" s="4" t="s">
         <v>110</v>
       </c>
@@ -14539,7 +14550,7 @@
         <v>539.70903225806455</v>
       </c>
     </row>
-    <row r="226" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A226" s="4" t="s">
         <v>110</v>
       </c>
@@ -14592,7 +14603,7 @@
         <v>585.62967741935483</v>
       </c>
     </row>
-    <row r="227" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A227" s="4" t="s">
         <v>110</v>
       </c>
@@ -14645,7 +14656,7 @@
         <v>79.359677419354838</v>
       </c>
     </row>
-    <row r="228" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A228" s="4" t="s">
         <v>110</v>
       </c>
@@ -14698,7 +14709,7 @@
         <v>486.09451612903229</v>
       </c>
     </row>
-    <row r="229" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A229" s="4" t="s">
         <v>110</v>
       </c>
@@ -14751,7 +14762,7 @@
         <v>6018.8180645161283</v>
       </c>
     </row>
-    <row r="230" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A230" s="4" t="s">
         <v>110</v>
       </c>
@@ -14804,7 +14815,7 @@
         <v>2483.2987096774191</v>
       </c>
     </row>
-    <row r="231" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A231" s="4" t="s">
         <v>110</v>
       </c>
@@ -14857,7 +14868,7 @@
         <v>28959.753870967746</v>
       </c>
     </row>
-    <row r="232" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A232" s="4" t="s">
         <v>110</v>
       </c>
@@ -14910,7 +14921,7 @@
         <v>630.94322580645155</v>
       </c>
     </row>
-    <row r="233" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A233" s="4" t="s">
         <v>110</v>
       </c>
@@ -14963,7 +14974,7 @@
         <v>225.88580645161289</v>
       </c>
     </row>
-    <row r="234" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A234" s="4" t="s">
         <v>110</v>
       </c>
@@ -15016,7 +15027,7 @@
         <v>300.07258064516128</v>
       </c>
     </row>
-    <row r="235" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A235" s="4" t="s">
         <v>110</v>
       </c>
@@ -15069,7 +15080,7 @@
         <v>219.88580645161289</v>
       </c>
     </row>
-    <row r="236" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A236" s="4" t="s">
         <v>110</v>
       </c>
@@ -15122,7 +15133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A237" s="4" t="s">
         <v>110</v>
       </c>
@@ -15175,7 +15186,7 @@
         <v>1915.2125806451611</v>
       </c>
     </row>
-    <row r="238" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A238" s="4" t="s">
         <v>353</v>
       </c>
@@ -15228,7 +15239,7 @@
         <v>452.93161290322575</v>
       </c>
     </row>
-    <row r="239" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A239" s="4" t="s">
         <v>353</v>
       </c>
@@ -15281,7 +15292,7 @@
         <v>133.33806451612901</v>
       </c>
     </row>
-    <row r="240" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A240" s="4" t="s">
         <v>353</v>
       </c>
@@ -15334,7 +15345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A241" s="4" t="s">
         <v>360</v>
       </c>
@@ -15387,7 +15398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A242" s="4" t="s">
         <v>360</v>
       </c>
@@ -15440,7 +15451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A243" s="4" t="s">
         <v>360</v>
       </c>
@@ -15493,7 +15504,7 @@
         <v>89.031935483870967</v>
       </c>
     </row>
-    <row r="244" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A244" s="4" t="s">
         <v>360</v>
       </c>
@@ -15546,7 +15557,7 @@
         <v>367.47419354838706</v>
       </c>
     </row>
-    <row r="245" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A245" s="4" t="s">
         <v>360</v>
       </c>
@@ -15599,7 +15610,7 @@
         <v>27.87709677419355</v>
       </c>
     </row>
-    <row r="246" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A246" s="4" t="s">
         <v>360</v>
       </c>
@@ -15652,7 +15663,7 @@
         <v>1.685483870967742</v>
       </c>
     </row>
-    <row r="247" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A247" s="4" t="s">
         <v>360</v>
       </c>
@@ -15705,7 +15716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A248" s="4" t="s">
         <v>360</v>
       </c>
@@ -15758,7 +15769,7 @@
         <v>2.4925806451612904</v>
       </c>
     </row>
-    <row r="249" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A249" s="4" t="s">
         <v>360</v>
       </c>
@@ -15811,7 +15822,7 @@
         <v>4.8603225806451613</v>
       </c>
     </row>
-    <row r="250" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A250" s="4" t="s">
         <v>360</v>
       </c>
@@ -15864,7 +15875,7 @@
         <v>25.683870967741935</v>
       </c>
     </row>
-    <row r="251" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A251" s="4" t="s">
         <v>360</v>
       </c>
@@ -15917,7 +15928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A252" s="4" t="s">
         <v>360</v>
       </c>
@@ -15970,7 +15981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A253" s="4" t="s">
         <v>360</v>
       </c>
@@ -16023,7 +16034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A254" s="4" t="s">
         <v>360</v>
       </c>
@@ -16076,7 +16087,7 @@
         <v>18.509354838709676</v>
       </c>
     </row>
-    <row r="255" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A255" s="4" t="s">
         <v>360</v>
       </c>
@@ -16129,7 +16140,7 @@
         <v>202.5825806451613</v>
       </c>
     </row>
-    <row r="256" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A256" s="4" t="s">
         <v>360</v>
       </c>
@@ -16182,7 +16193,7 @@
         <v>674.26548387096773</v>
       </c>
     </row>
-    <row r="257" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A257" s="4" t="s">
         <v>360</v>
       </c>
@@ -16235,7 +16246,7 @@
         <v>33.672903225806451</v>
       </c>
     </row>
-    <row r="258" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A258" s="4" t="s">
         <v>360</v>
       </c>
@@ -16288,7 +16299,7 @@
         <v>31.592580645161291</v>
       </c>
     </row>
-    <row r="259" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A259" s="4" t="s">
         <v>360</v>
       </c>
@@ -16341,7 +16352,7 @@
         <v>73.288709677419348</v>
       </c>
     </row>
-    <row r="260" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A260" s="4" t="s">
         <v>360</v>
       </c>
@@ -16394,7 +16405,7 @@
         <v>1850.4335483870968</v>
       </c>
     </row>
-    <row r="261" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A261" s="4" t="s">
         <v>360</v>
       </c>
@@ -16447,7 +16458,7 @@
         <v>751.91709677419351</v>
       </c>
     </row>
-    <row r="262" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A262" s="4" t="s">
         <v>360</v>
       </c>
@@ -16500,7 +16511,7 @@
         <v>20827.438064516129</v>
       </c>
     </row>
-    <row r="263" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A263" s="4" t="s">
         <v>360</v>
       </c>
@@ -16553,7 +16564,7 @@
         <v>42.831612903225803</v>
       </c>
     </row>
-    <row r="264" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A264" s="4" t="s">
         <v>360</v>
       </c>
@@ -16606,7 +16617,7 @@
         <v>3.5148387096774192</v>
       </c>
     </row>
-    <row r="265" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A265" s="4" t="s">
         <v>395</v>
       </c>
@@ -16659,7 +16670,7 @@
         <v>0.34903225806451615</v>
       </c>
     </row>
-    <row r="266" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A266" s="4" t="s">
         <v>395</v>
       </c>
@@ -16712,7 +16723,7 @@
         <v>0.10096774193548387</v>
       </c>
     </row>
-    <row r="267" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A267" s="4" t="s">
         <v>402</v>
       </c>
@@ -16765,7 +16776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A268" s="4" t="s">
         <v>402</v>
       </c>
@@ -16818,7 +16829,7 @@
         <v>137.54838709677421</v>
       </c>
     </row>
-    <row r="269" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A269" s="4" t="s">
         <v>402</v>
       </c>
@@ -16871,7 +16882,7 @@
         <v>52.019677419354835</v>
       </c>
     </row>
-    <row r="270" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A270" s="4" t="s">
         <v>408</v>
       </c>
@@ -16924,7 +16935,7 @@
         <v>2816.2651612903228</v>
       </c>
     </row>
-    <row r="271" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A271" s="4" t="s">
         <v>412</v>
       </c>
@@ -16977,7 +16988,7 @@
         <v>794.49064516129033</v>
       </c>
     </row>
-    <row r="272" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A272" s="4" t="s">
         <v>412</v>
       </c>
@@ -17030,7 +17041,7 @@
         <v>1249.51</v>
       </c>
     </row>
-    <row r="273" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A273" s="4" t="s">
         <v>412</v>
       </c>
@@ -17083,7 +17094,7 @@
         <v>249.00838709677421</v>
       </c>
     </row>
-    <row r="274" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A274" s="4" t="s">
         <v>412</v>
       </c>
@@ -17136,7 +17147,7 @@
         <v>1690.8109677419354</v>
       </c>
     </row>
-    <row r="275" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A275" s="4" t="s">
         <v>412</v>
       </c>
@@ -17189,7 +17200,7 @@
         <v>429.43387096774194</v>
       </c>
     </row>
-    <row r="276" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A276" s="4" t="s">
         <v>412</v>
       </c>
@@ -17242,7 +17253,7 @@
         <v>3122.1996774193549</v>
       </c>
     </row>
-    <row r="277" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A277" s="4" t="s">
         <v>412</v>
       </c>
@@ -17295,7 +17306,7 @@
         <v>274.21806451612906</v>
       </c>
     </row>
-    <row r="278" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A278" s="4" t="s">
         <v>412</v>
       </c>
@@ -17348,7 +17359,7 @@
         <v>98.889354838709679</v>
       </c>
     </row>
-    <row r="279" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A279" s="4" t="s">
         <v>412</v>
       </c>
@@ -17401,7 +17412,7 @@
         <v>175.09032258064514</v>
       </c>
     </row>
-    <row r="280" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A280" s="4" t="s">
         <v>412</v>
       </c>
@@ -17454,7 +17465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A281" s="4" t="s">
         <v>412</v>
       </c>
@@ -17507,7 +17518,7 @@
         <v>43.345806451612901</v>
       </c>
     </row>
-    <row r="282" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A282" s="4" t="s">
         <v>412</v>
       </c>
@@ -17560,7 +17571,7 @@
         <v>175.13774193548389</v>
       </c>
     </row>
-    <row r="283" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A283" s="4" t="s">
         <v>412</v>
       </c>
@@ -17613,7 +17624,7 @@
         <v>14.620000000000001</v>
       </c>
     </row>
-    <row r="284" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A284" s="4" t="s">
         <v>412</v>
       </c>
@@ -17666,7 +17677,7 @@
         <v>1095.07</v>
       </c>
     </row>
-    <row r="285" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A285" s="4" t="s">
         <v>412</v>
       </c>
@@ -17719,7 +17730,7 @@
         <v>53.19483870967742</v>
       </c>
     </row>
-    <row r="286" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A286" s="4" t="s">
         <v>412</v>
       </c>
@@ -17772,7 +17783,7 @@
         <v>4400.2087096774194</v>
       </c>
     </row>
-    <row r="287" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A287" s="4" t="s">
         <v>412</v>
       </c>
@@ -17825,7 +17836,7 @@
         <v>2847.719032258065</v>
       </c>
     </row>
-    <row r="288" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A288" s="4" t="s">
         <v>412</v>
       </c>
@@ -17878,7 +17889,7 @@
         <v>200.90451612903226</v>
       </c>
     </row>
-    <row r="289" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A289" s="4" t="s">
         <v>412</v>
       </c>
@@ -17931,7 +17942,7 @@
         <v>1105.1774193548388</v>
       </c>
     </row>
-    <row r="290" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A290" s="4" t="s">
         <v>412</v>
       </c>
@@ -17984,7 +17995,7 @@
         <v>380.14322580645165</v>
       </c>
     </row>
-    <row r="291" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A291" s="4" t="s">
         <v>412</v>
       </c>
@@ -18037,7 +18048,7 @@
         <v>114.84903225806453</v>
       </c>
     </row>
-    <row r="292" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A292" s="4" t="s">
         <v>412</v>
       </c>
@@ -18090,7 +18101,7 @@
         <v>1186.0487096774193</v>
       </c>
     </row>
-    <row r="293" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A293" s="4" t="s">
         <v>412</v>
       </c>
@@ -18143,7 +18154,7 @@
         <v>113.57548387096774</v>
       </c>
     </row>
-    <row r="294" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A294" s="4" t="s">
         <v>412</v>
       </c>
@@ -18196,7 +18207,7 @@
         <v>1821.0629032258064</v>
       </c>
     </row>
-    <row r="295" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A295" s="4" t="s">
         <v>412</v>
       </c>
@@ -18249,7 +18260,7 @@
         <v>526.33806451612907</v>
       </c>
     </row>
-    <row r="296" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A296" s="4" t="s">
         <v>412</v>
       </c>
@@ -18302,7 +18313,7 @@
         <v>685.40677419354836</v>
       </c>
     </row>
-    <row r="297" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A297" s="4" t="s">
         <v>412</v>
       </c>
@@ -18355,7 +18366,7 @@
         <v>383.93838709677419</v>
       </c>
     </row>
-    <row r="298" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A298" s="4" t="s">
         <v>412</v>
       </c>
@@ -18408,7 +18419,7 @@
         <v>1937.446451612903</v>
       </c>
     </row>
-    <row r="299" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A299" s="4" t="s">
         <v>453</v>
       </c>
@@ -18461,7 +18472,7 @@
         <v>157.57193548387096</v>
       </c>
     </row>
-    <row r="300" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A300" s="4" t="s">
         <v>453</v>
       </c>
@@ -18514,7 +18525,7 @@
         <v>2.0851612903225805</v>
       </c>
     </row>
-    <row r="301" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A301" s="4" t="s">
         <v>453</v>
       </c>
@@ -18567,7 +18578,7 @@
         <v>0.95129032258064516</v>
       </c>
     </row>
-    <row r="302" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A302" s="4" t="s">
         <v>453</v>
       </c>
@@ -18620,7 +18631,7 @@
         <v>1.0238709677419355</v>
       </c>
     </row>
-    <row r="303" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A303" s="4" t="s">
         <v>453</v>
       </c>
@@ -18673,7 +18684,7 @@
         <v>2.4854838709677418</v>
       </c>
     </row>
-    <row r="304" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A304" s="4" t="s">
         <v>462</v>
       </c>
@@ -18726,7 +18737,7 @@
         <v>12132.312258064516</v>
       </c>
     </row>
-    <row r="305" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A305" s="4" t="s">
         <v>462</v>
       </c>
@@ -18779,7 +18790,7 @@
         <v>42612.364193548383</v>
       </c>
     </row>
-    <row r="306" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A306" s="4" t="s">
         <v>462</v>
       </c>
@@ -18832,7 +18843,7 @@
         <v>48108.182903225803</v>
       </c>
     </row>
-    <row r="307" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A307" s="4" t="s">
         <v>462</v>
       </c>
@@ -18885,7 +18896,7 @@
         <v>376.3083870967742</v>
       </c>
     </row>
-    <row r="308" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A308" s="4" t="s">
         <v>462</v>
       </c>
@@ -18938,7 +18949,7 @@
         <v>242.73967741935485</v>
       </c>
     </row>
-    <row r="309" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A309" s="4" t="s">
         <v>462</v>
       </c>
@@ -18991,7 +19002,7 @@
         <v>227.80451612903227</v>
       </c>
     </row>
-    <row r="310" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A310" s="4" t="s">
         <v>462</v>
       </c>
@@ -19044,7 +19055,7 @@
         <v>76.187096774193549</v>
       </c>
     </row>
-    <row r="311" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A311" s="4" t="s">
         <v>462</v>
       </c>
@@ -19097,7 +19108,7 @@
         <v>222.70741935483872</v>
       </c>
     </row>
-    <row r="312" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A312" s="4" t="s">
         <v>462</v>
       </c>
@@ -19150,7 +19161,7 @@
         <v>303.82225806451612</v>
       </c>
     </row>
-    <row r="313" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A313" s="4" t="s">
         <v>462</v>
       </c>
@@ -19203,7 +19214,7 @@
         <v>305.40677419354842</v>
       </c>
     </row>
-    <row r="314" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" s="4" t="s">
         <v>462</v>
       </c>
@@ -19256,7 +19267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A315" s="4" t="s">
         <v>462</v>
       </c>
@@ -19309,7 +19320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A316" s="4" t="s">
         <v>462</v>
       </c>
@@ -19362,7 +19373,7 @@
         <v>3237.7512903225811</v>
       </c>
     </row>
-    <row r="317" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A317" s="4" t="s">
         <v>462</v>
       </c>
@@ -19415,7 +19426,7 @@
         <v>5582.3929032258065</v>
       </c>
     </row>
-    <row r="318" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A318" s="4" t="s">
         <v>462</v>
       </c>
@@ -19468,7 +19479,7 @@
         <v>1534.903870967742</v>
       </c>
     </row>
-    <row r="319" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A319" s="4" t="s">
         <v>462</v>
       </c>
@@ -19521,7 +19532,7 @@
         <v>998.19225806451607</v>
       </c>
     </row>
-    <row r="320" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A320" s="4" t="s">
         <v>462</v>
       </c>
@@ -19574,7 +19585,7 @@
         <v>1678.758064516129</v>
       </c>
     </row>
-    <row r="321" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A321" s="4" t="s">
         <v>462</v>
       </c>
@@ -19627,7 +19638,7 @@
         <v>422.95419354838708</v>
       </c>
     </row>
-    <row r="322" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A322" s="4" t="s">
         <v>462</v>
       </c>
@@ -19680,7 +19691,7 @@
         <v>413.2161290322581</v>
       </c>
     </row>
-    <row r="323" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A323" s="4" t="s">
         <v>462</v>
       </c>
@@ -19733,7 +19744,7 @@
         <v>3132.2212903225804</v>
       </c>
     </row>
-    <row r="324" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A324" s="4" t="s">
         <v>462</v>
       </c>
@@ -19786,7 +19797,7 @@
         <v>72496.146129032248</v>
       </c>
     </row>
-    <row r="325" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A325" s="4" t="s">
         <v>462</v>
       </c>
@@ -19839,7 +19850,7 @@
         <v>340.06032258064516</v>
       </c>
     </row>
-    <row r="326" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A326" s="4" t="s">
         <v>462</v>
       </c>
@@ -19892,7 +19903,7 @@
         <v>2327.5938709677421</v>
       </c>
     </row>
-    <row r="327" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" s="4" t="s">
         <v>462</v>
       </c>
@@ -19945,7 +19956,7 @@
         <v>2550.5087096774196</v>
       </c>
     </row>
-    <row r="328" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A328" s="4" t="s">
         <v>462</v>
       </c>
@@ -19998,7 +20009,7 @@
         <v>774.48354838709679</v>
       </c>
     </row>
-    <row r="329" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A329" s="4" t="s">
         <v>462</v>
       </c>
@@ -20051,7 +20062,7 @@
         <v>19041.383870967744</v>
       </c>
     </row>
-    <row r="330" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A330" s="4" t="s">
         <v>462</v>
       </c>
@@ -20104,7 +20115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A331" s="4" t="s">
         <v>462</v>
       </c>
@@ -20157,7 +20168,7 @@
         <v>2663.4225806451614</v>
       </c>
     </row>
-    <row r="332" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A332" s="4" t="s">
         <v>462</v>
       </c>
@@ -20210,7 +20221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A333" s="4" t="s">
         <v>462</v>
       </c>
@@ -20263,7 +20274,7 @@
         <v>2320.2996774193548</v>
       </c>
     </row>
-    <row r="334" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A334" s="4" t="s">
         <v>462</v>
       </c>
@@ -20316,7 +20327,7 @@
         <v>2016.1609677419353</v>
       </c>
     </row>
-    <row r="335" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A335" s="4" t="s">
         <v>462</v>
       </c>
@@ -20369,7 +20380,7 @@
         <v>951.14354838709676</v>
       </c>
     </row>
-    <row r="336" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A336" s="4" t="s">
         <v>462</v>
       </c>
@@ -20422,7 +20433,7 @@
         <v>1730.0383870967742</v>
       </c>
     </row>
-    <row r="337" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A337" s="4" t="s">
         <v>462</v>
       </c>
@@ -20475,7 +20486,7 @@
         <v>650.62064516129033</v>
       </c>
     </row>
-    <row r="338" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A338" s="4" t="s">
         <v>462</v>
       </c>
@@ -20528,7 +20539,7 @@
         <v>1215.726451612903</v>
       </c>
     </row>
-    <row r="339" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A339" s="4" t="s">
         <v>462</v>
       </c>
@@ -20581,7 +20592,7 @@
         <v>1341.6151612903225</v>
       </c>
     </row>
-    <row r="340" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A340" s="4" t="s">
         <v>462</v>
       </c>
@@ -20634,7 +20645,7 @@
         <v>118.70129032258063</v>
       </c>
     </row>
-    <row r="341" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A341" s="4" t="s">
         <v>462</v>
       </c>
@@ -20687,7 +20698,7 @@
         <v>158.83161290322579</v>
       </c>
     </row>
-    <row r="342" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A342" s="4" t="s">
         <v>462</v>
       </c>
@@ -20740,7 +20751,7 @@
         <v>314.77935483870965</v>
       </c>
     </row>
-    <row r="343" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" s="4" t="s">
         <v>462</v>
       </c>
@@ -20793,7 +20804,7 @@
         <v>120.56709677419354</v>
       </c>
     </row>
-    <row r="344" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" s="4" t="s">
         <v>462</v>
       </c>
@@ -20846,7 +20857,7 @@
         <v>209.81161290322581</v>
       </c>
     </row>
-    <row r="345" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" s="4" t="s">
         <v>462</v>
       </c>
@@ -20899,7 +20910,7 @@
         <v>3484.6264516129031</v>
       </c>
     </row>
-    <row r="346" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" s="4" t="s">
         <v>462</v>
       </c>
@@ -20952,7 +20963,7 @@
         <v>122560.08935483871</v>
       </c>
     </row>
-    <row r="347" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A347" s="4" t="s">
         <v>462</v>
       </c>
@@ -21005,7 +21016,7 @@
         <v>1007.3009677419356</v>
       </c>
     </row>
-    <row r="348" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" s="4" t="s">
         <v>462</v>
       </c>
@@ -21058,7 +21069,7 @@
         <v>1074.1941935483869</v>
       </c>
     </row>
-    <row r="349" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A349" s="4" t="s">
         <v>462</v>
       </c>
@@ -21111,7 +21122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" s="4" t="s">
         <v>462</v>
       </c>
@@ -21164,7 +21175,7 @@
         <v>2731.9780645161291</v>
       </c>
     </row>
-    <row r="351" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" s="4" t="s">
         <v>462</v>
       </c>
@@ -21217,7 +21228,7 @@
         <v>79.009677419354844</v>
       </c>
     </row>
-    <row r="352" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" s="4" t="s">
         <v>462</v>
       </c>
@@ -21270,7 +21281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" s="4" t="s">
         <v>462</v>
       </c>
@@ -21323,7 +21334,7 @@
         <v>44613.312258064514</v>
       </c>
     </row>
-    <row r="354" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" s="4" t="s">
         <v>462</v>
       </c>
@@ -21376,7 +21387,7 @@
         <v>825.78903225806448</v>
       </c>
     </row>
-    <row r="355" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" s="4" t="s">
         <v>462</v>
       </c>
@@ -21429,7 +21440,7 @@
         <v>9322.7806451612905</v>
       </c>
     </row>
-    <row r="356" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" s="4" t="s">
         <v>462</v>
       </c>
@@ -21482,7 +21493,7 @@
         <v>1473.5974193548386</v>
       </c>
     </row>
-    <row r="357" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" s="4" t="s">
         <v>462</v>
       </c>
@@ -21535,7 +21546,7 @@
         <v>699.09903225806454</v>
       </c>
     </row>
-    <row r="358" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" s="4" t="s">
         <v>462</v>
       </c>
@@ -21588,7 +21599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" s="4" t="s">
         <v>462</v>
       </c>
@@ -21641,7 +21652,7 @@
         <v>1538.4803225806452</v>
       </c>
     </row>
-    <row r="360" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" s="4" t="s">
         <v>462</v>
       </c>
@@ -21694,7 +21705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" s="4" t="s">
         <v>462</v>
       </c>
@@ -21747,7 +21758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" s="4" t="s">
         <v>462</v>
       </c>
@@ -21800,7 +21811,7 @@
         <v>298.24935483870968</v>
       </c>
     </row>
-    <row r="363" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A363" s="4" t="s">
         <v>462</v>
       </c>
@@ -21853,7 +21864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A364" s="4" t="s">
         <v>462</v>
       </c>
@@ -21906,7 +21917,7 @@
         <v>1353.0345161290322</v>
       </c>
     </row>
-    <row r="365" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A365" s="4" t="s">
         <v>462</v>
       </c>
@@ -21959,7 +21970,7 @@
         <v>554.27612903225804</v>
       </c>
     </row>
-    <row r="366" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A366" s="4" t="s">
         <v>462</v>
       </c>
@@ -22012,7 +22023,7 @@
         <v>323.82</v>
       </c>
     </row>
-    <row r="367" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A367" s="4" t="s">
         <v>462</v>
       </c>
@@ -22065,7 +22076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A368" s="4" t="s">
         <v>462</v>
       </c>
@@ -22118,7 +22129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A369" s="4" t="s">
         <v>462</v>
       </c>
@@ -22171,7 +22182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A370" s="4" t="s">
         <v>462</v>
       </c>
@@ -22224,7 +22235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A371" s="4" t="s">
         <v>462</v>
       </c>
@@ -22277,7 +22288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A372" s="4" t="s">
         <v>462</v>
       </c>
@@ -22330,7 +22341,7 @@
         <v>4164.7880645161295</v>
       </c>
     </row>
-    <row r="373" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A373" s="4" t="s">
         <v>462</v>
       </c>
@@ -22383,7 +22394,7 @@
         <v>292.18225806451613</v>
       </c>
     </row>
-    <row r="374" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A374" s="4" t="s">
         <v>462</v>
       </c>
@@ -22436,7 +22447,7 @@
         <v>673.0264516129032</v>
       </c>
     </row>
-    <row r="375" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A375" s="4" t="s">
         <v>462</v>
       </c>
@@ -22489,7 +22500,7 @@
         <v>935.0396774193548</v>
       </c>
     </row>
-    <row r="376" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A376" s="4" t="s">
         <v>462</v>
       </c>
@@ -22542,7 +22553,7 @@
         <v>2433.6529032258063</v>
       </c>
     </row>
-    <row r="377" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A377" s="4" t="s">
         <v>462</v>
       </c>
@@ -22595,7 +22606,7 @@
         <v>14.032903225806452</v>
       </c>
     </row>
-    <row r="378" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A378" s="4" t="s">
         <v>462</v>
       </c>
@@ -22648,7 +22659,7 @@
         <v>210.46096774193549</v>
       </c>
     </row>
-    <row r="379" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A379" s="4" t="s">
         <v>462</v>
       </c>
@@ -22701,7 +22712,7 @@
         <v>6.7438709677419357</v>
       </c>
     </row>
-    <row r="380" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A380" s="4" t="s">
         <v>462</v>
       </c>
@@ -22754,7 +22765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A381" s="4" t="s">
         <v>462</v>
       </c>
@@ -22807,7 +22818,7 @@
         <v>2158.7035483870968</v>
       </c>
     </row>
-    <row r="382" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A382" s="4" t="s">
         <v>462</v>
       </c>
@@ -22860,7 +22871,7 @@
         <v>1734.1522580645162</v>
       </c>
     </row>
-    <row r="383" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A383" s="4" t="s">
         <v>462</v>
       </c>
@@ -22913,7 +22924,7 @@
         <v>146.00709677419357</v>
       </c>
     </row>
-    <row r="384" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A384" s="4" t="s">
         <v>564</v>
       </c>
@@ -22966,7 +22977,7 @@
         <v>232.44516129032257</v>
       </c>
     </row>
-    <row r="385" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A385" s="4" t="s">
         <v>568</v>
       </c>
@@ -23019,7 +23030,7 @@
         <v>349.38451612903225</v>
       </c>
     </row>
-    <row r="386" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A386" s="4" t="s">
         <v>568</v>
       </c>
@@ -23072,7 +23083,7 @@
         <v>54.002258064516127</v>
       </c>
     </row>
-    <row r="387" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A387" s="4" t="s">
         <v>568</v>
       </c>
@@ -23125,7 +23136,7 @@
         <v>2.2903225806451613E-2</v>
       </c>
     </row>
-    <row r="388" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A388" s="4" t="s">
         <v>568</v>
       </c>
@@ -23178,7 +23189,7 @@
         <v>135.85806451612905</v>
       </c>
     </row>
-    <row r="389" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A389" s="4" t="s">
         <v>568</v>
       </c>
@@ -23231,7 +23242,7 @@
         <v>1753.7012903225809</v>
       </c>
     </row>
-    <row r="390" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A390" s="4" t="s">
         <v>580</v>
       </c>
@@ -23284,7 +23295,7 @@
         <v>3599.5577419354836</v>
       </c>
     </row>
-    <row r="391" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A391" s="4" t="s">
         <v>580</v>
       </c>
@@ -23337,7 +23348,7 @@
         <v>247.97709677419354</v>
       </c>
     </row>
-    <row r="392" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A392" s="4" t="s">
         <v>580</v>
       </c>
@@ -23390,7 +23401,7 @@
         <v>1372.9583870967742</v>
       </c>
     </row>
-    <row r="393" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A393" s="4" t="s">
         <v>580</v>
       </c>
@@ -23443,7 +23454,7 @@
         <v>182.85419354838709</v>
       </c>
     </row>
-    <row r="394" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A394" s="4" t="s">
         <v>580</v>
       </c>
@@ -23496,7 +23507,7 @@
         <v>2183.3787096774195</v>
       </c>
     </row>
-    <row r="395" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A395" s="4" t="s">
         <v>580</v>
       </c>
@@ -23549,7 +23560,7 @@
         <v>106.83322580645161</v>
       </c>
     </row>
-    <row r="396" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A396" s="4" t="s">
         <v>580</v>
       </c>
@@ -23602,7 +23613,7 @@
         <v>62.399677419354845</v>
       </c>
     </row>
-    <row r="397" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A397" s="4" t="s">
         <v>580</v>
       </c>
@@ -23655,7 +23666,7 @@
         <v>200.80483870967743</v>
       </c>
     </row>
-    <row r="398" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A398" s="4" t="s">
         <v>580</v>
       </c>
@@ -23708,7 +23719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A399" s="4" t="s">
         <v>580</v>
       </c>
@@ -23761,7 +23772,7 @@
         <v>858.87645161290322</v>
       </c>
     </row>
-    <row r="400" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A400" s="4" t="s">
         <v>580</v>
       </c>
@@ -23814,7 +23825,7 @@
         <v>5767.7451612903224</v>
       </c>
     </row>
-    <row r="401" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A401" s="4" t="s">
         <v>580</v>
       </c>
@@ -23867,7 +23878,7 @@
         <v>489.13870967741934</v>
       </c>
     </row>
-    <row r="402" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A402" s="4" t="s">
         <v>580</v>
       </c>
@@ -23920,7 +23931,7 @@
         <v>492.47612903225809</v>
       </c>
     </row>
-    <row r="403" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A403" s="4" t="s">
         <v>580</v>
       </c>
@@ -23973,7 +23984,7 @@
         <v>3272.0287096774196</v>
       </c>
     </row>
-    <row r="404" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A404" s="4" t="s">
         <v>580</v>
       </c>
@@ -24026,7 +24037,7 @@
         <v>360.85193548387099</v>
       </c>
     </row>
-    <row r="405" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A405" s="4" t="s">
         <v>580</v>
       </c>
@@ -24079,7 +24090,7 @@
         <v>106.83387096774193</v>
       </c>
     </row>
-    <row r="406" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A406" s="4" t="s">
         <v>580</v>
       </c>
@@ -24132,7 +24143,7 @@
         <v>1334.4938709677419</v>
       </c>
     </row>
-    <row r="407" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A407" s="4" t="s">
         <v>580</v>
       </c>
@@ -24185,7 +24196,7 @@
         <v>268.34645161290319</v>
       </c>
     </row>
-    <row r="408" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A408" s="4" t="s">
         <v>580</v>
       </c>
@@ -24238,7 +24249,7 @@
         <v>28.845806451612905</v>
       </c>
     </row>
-    <row r="409" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A409" s="4" t="s">
         <v>580</v>
       </c>
@@ -24291,7 +24302,7 @@
         <v>458.27580645161288</v>
       </c>
     </row>
-    <row r="410" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A410" s="4" t="s">
         <v>580</v>
       </c>
@@ -24344,7 +24355,7 @@
         <v>264.61290000000002</v>
       </c>
     </row>
-    <row r="411" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A411" s="4" t="s">
         <v>580</v>
       </c>
@@ -24397,7 +24408,7 @@
         <v>243.75838709677421</v>
       </c>
     </row>
-    <row r="412" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A412" s="4" t="s">
         <v>580</v>
       </c>
@@ -24450,7 +24461,7 @@
         <v>342.55806451612904</v>
       </c>
     </row>
-    <row r="413" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A413" s="4" t="s">
         <v>580</v>
       </c>
@@ -24503,7 +24514,7 @@
         <v>7821.1803225806452</v>
       </c>
     </row>
-    <row r="414" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A414" s="4" t="s">
         <v>580</v>
       </c>
@@ -24556,7 +24567,7 @@
         <v>430.74967741935484</v>
       </c>
     </row>
-    <row r="415" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A415" s="4" t="s">
         <v>580</v>
       </c>
@@ -24609,7 +24620,7 @@
         <v>383.16774193548389</v>
       </c>
     </row>
-    <row r="416" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A416" s="4" t="s">
         <v>618</v>
       </c>
@@ -24662,7 +24673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A417" s="4" t="s">
         <v>618</v>
       </c>
@@ -24715,7 +24726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A418" s="4" t="s">
         <v>618</v>
       </c>
@@ -24768,7 +24779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A419" s="4" t="s">
         <v>618</v>
       </c>
@@ -24821,7 +24832,7 @@
         <v>13584.31741935484</v>
       </c>
     </row>
-    <row r="420" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A420" s="4" t="s">
         <v>618</v>
       </c>
@@ -24874,7 +24885,7 @@
         <v>31320.664516129033</v>
       </c>
     </row>
-    <row r="421" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A421" s="4" t="s">
         <v>618</v>
       </c>
@@ -24927,7 +24938,7 @@
         <v>3973.4235483870971</v>
       </c>
     </row>
-    <row r="422" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A422" s="4" t="s">
         <v>618</v>
       </c>
@@ -24980,7 +24991,7 @@
         <v>0.54129032258064524</v>
       </c>
     </row>
-    <row r="423" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A423" s="4" t="s">
         <v>618</v>
       </c>
@@ -25033,7 +25044,7 @@
         <v>1.3261290322580646</v>
       </c>
     </row>
-    <row r="424" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A424" s="4" t="s">
         <v>618</v>
       </c>
@@ -25086,7 +25097,7 @@
         <v>28.36032258064516</v>
       </c>
     </row>
-    <row r="425" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A425" s="4" t="s">
         <v>618</v>
       </c>
@@ -25139,7 +25150,7 @@
         <v>3.995483870967742</v>
       </c>
     </row>
-    <row r="426" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A426" s="4" t="s">
         <v>618</v>
       </c>
@@ -25192,7 +25203,7 @@
         <v>52.607096774193543</v>
       </c>
     </row>
-    <row r="427" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A427" s="4" t="s">
         <v>618</v>
       </c>
@@ -25245,7 +25256,7 @@
         <v>34.030645161290323</v>
       </c>
     </row>
-    <row r="428" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A428" s="4" t="s">
         <v>618</v>
       </c>
@@ -25298,7 +25309,7 @@
         <v>332.08064516129031</v>
       </c>
     </row>
-    <row r="429" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A429" s="4" t="s">
         <v>618</v>
       </c>
@@ -25351,7 +25362,7 @@
         <v>4845.5009677419357</v>
       </c>
     </row>
-    <row r="430" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A430" s="4" t="s">
         <v>618</v>
       </c>
@@ -25404,7 +25415,7 @@
         <v>1697.7203225806452</v>
       </c>
     </row>
-    <row r="431" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A431" s="4" t="s">
         <v>618</v>
       </c>
@@ -25457,7 +25468,7 @@
         <v>223.7516129032258</v>
       </c>
     </row>
-    <row r="432" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A432" s="4" t="s">
         <v>618</v>
       </c>
@@ -25510,7 +25521,7 @@
         <v>365.70258064516133</v>
       </c>
     </row>
-    <row r="433" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A433" s="4" t="s">
         <v>618</v>
       </c>
@@ -25563,7 +25574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A434" s="4" t="s">
         <v>618</v>
       </c>
@@ -25616,7 +25627,7 @@
         <v>268.17</v>
       </c>
     </row>
-    <row r="435" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A435" s="4" t="s">
         <v>618</v>
       </c>
@@ -25669,7 +25680,7 @@
         <v>2588.554193548387</v>
       </c>
     </row>
-    <row r="436" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A436" s="4" t="s">
         <v>618</v>
       </c>
@@ -25722,7 +25733,7 @@
         <v>40.578709677419354</v>
       </c>
     </row>
-    <row r="437" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A437" s="4" t="s">
         <v>618</v>
       </c>
@@ -25775,7 +25786,7 @@
         <v>194.30193548387095</v>
       </c>
     </row>
-    <row r="438" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A438" s="4" t="s">
         <v>618</v>
       </c>
@@ -25828,7 +25839,7 @@
         <v>548.49903225806452</v>
       </c>
     </row>
-    <row r="439" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A439" s="4" t="s">
         <v>618</v>
       </c>
@@ -25881,7 +25892,7 @@
         <v>7.3738709677419356</v>
       </c>
     </row>
-    <row r="440" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A440" s="4" t="s">
         <v>618</v>
       </c>
@@ -25934,7 +25945,7 @@
         <v>1111.3380645161292</v>
       </c>
     </row>
-    <row r="441" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A441" s="4" t="s">
         <v>618</v>
       </c>
@@ -25987,7 +25998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A442" s="4" t="s">
         <v>618</v>
       </c>
@@ -26040,7 +26051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A443" s="4" t="s">
         <v>618</v>
       </c>
@@ -26093,7 +26104,7 @@
         <v>106.55612903225806</v>
       </c>
     </row>
-    <row r="444" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A444" s="4" t="s">
         <v>618</v>
       </c>
@@ -26146,7 +26157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A445" s="4" t="s">
         <v>618</v>
       </c>
@@ -26199,7 +26210,7 @@
         <v>852.27741935483868</v>
       </c>
     </row>
-    <row r="446" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A446" s="4" t="s">
         <v>618</v>
       </c>
@@ -26252,7 +26263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A447" s="4" t="s">
         <v>618</v>
       </c>
@@ -26305,7 +26316,7 @@
         <v>1181.6012903225806</v>
       </c>
     </row>
-    <row r="448" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A448" s="4" t="s">
         <v>618</v>
       </c>
@@ -26358,7 +26369,7 @@
         <v>194.98548387096776</v>
       </c>
     </row>
-    <row r="449" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A449" s="4" t="s">
         <v>618</v>
       </c>
@@ -26411,7 +26422,7 @@
         <v>755.5248387096774</v>
       </c>
     </row>
-    <row r="450" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A450" s="4" t="s">
         <v>673</v>
       </c>
@@ -26464,7 +26475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A451" s="4" t="s">
         <v>673</v>
       </c>
@@ -26517,7 +26528,7 @@
         <v>6.3735483870967746</v>
       </c>
     </row>
-    <row r="452" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A452" s="4" t="s">
         <v>673</v>
       </c>
@@ -26570,7 +26581,7 @@
         <v>30.161290322580644</v>
       </c>
     </row>
-    <row r="453" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A453" s="4" t="s">
         <v>673</v>
       </c>
@@ -26623,7 +26634,7 @@
         <v>6.3870967741935486E-2</v>
       </c>
     </row>
-    <row r="454" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A454" s="4" t="s">
         <v>681</v>
       </c>
@@ -26676,7 +26687,7 @@
         <v>26.46</v>
       </c>
     </row>
-    <row r="455" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A455" s="4" t="s">
         <v>681</v>
       </c>
@@ -26729,7 +26740,7 @@
         <v>124.79967741935484</v>
       </c>
     </row>
-    <row r="456" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A456" s="4" t="s">
         <v>681</v>
       </c>
@@ -26782,7 +26793,7 @@
         <v>515.67741935483866</v>
       </c>
     </row>
-    <row r="457" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A457" s="4" t="s">
         <v>681</v>
       </c>
@@ -26835,7 +26846,7 @@
         <v>8.9616129032258058</v>
       </c>
     </row>
-    <row r="458" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A458" s="4" t="s">
         <v>681</v>
       </c>
@@ -26888,7 +26899,7 @@
         <v>6213.7209677419351</v>
       </c>
     </row>
-    <row r="459" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A459" s="4" t="s">
         <v>681</v>
       </c>
@@ -26941,7 +26952,7 @@
         <v>2344.8506451612902</v>
       </c>
     </row>
-    <row r="460" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A460" s="4" t="s">
         <v>681</v>
       </c>
@@ -26994,7 +27005,7 @@
         <v>253.29129032258064</v>
       </c>
     </row>
-    <row r="461" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A461" s="4" t="s">
         <v>681</v>
       </c>
@@ -27047,7 +27058,7 @@
         <v>257.25225806451613</v>
       </c>
     </row>
-    <row r="462" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A462" s="4" t="s">
         <v>681</v>
       </c>
@@ -27100,7 +27111,7 @@
         <v>1086.7006451612904</v>
       </c>
     </row>
-    <row r="463" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A463" s="4" t="s">
         <v>681</v>
       </c>
@@ -27153,7 +27164,7 @@
         <v>425.31096774193549</v>
       </c>
     </row>
-    <row r="464" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A464" s="4" t="s">
         <v>681</v>
       </c>
@@ -27206,7 +27217,7 @@
         <v>31.315483870967743</v>
       </c>
     </row>
-    <row r="465" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A465" s="4" t="s">
         <v>681</v>
       </c>
@@ -27259,7 +27270,7 @@
         <v>485.82419354838709</v>
       </c>
     </row>
-    <row r="466" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A466" s="4" t="s">
         <v>681</v>
       </c>
@@ -27312,7 +27323,7 @@
         <v>24.088387096774195</v>
       </c>
     </row>
-    <row r="467" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A467" s="4" t="s">
         <v>681</v>
       </c>
@@ -27365,7 +27376,7 @@
         <v>235.45032258064515</v>
       </c>
     </row>
-    <row r="468" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A468" s="4" t="s">
         <v>681</v>
       </c>
@@ -27418,7 +27429,7 @@
         <v>47.537741935483872</v>
       </c>
     </row>
-    <row r="469" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A469" s="4" t="s">
         <v>681</v>
       </c>
@@ -27471,7 +27482,7 @@
         <v>1620.6399999999999</v>
       </c>
     </row>
-    <row r="470" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A470" s="4" t="s">
         <v>681</v>
       </c>
@@ -27524,7 +27535,7 @@
         <v>107.89064516129032</v>
       </c>
     </row>
-    <row r="471" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A471" s="4" t="s">
         <v>681</v>
       </c>
@@ -27577,7 +27588,7 @@
         <v>194.82</v>
       </c>
     </row>
-    <row r="472" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:17" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A472" s="4" t="s">
         <v>681</v>
       </c>
@@ -27630,7 +27641,7 @@
         <v>78.551935483870977</v>
       </c>
     </row>
-    <row r="473" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:17" ht="22.5" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A473" s="7"/>
       <c r="B473" s="7"/>
       <c r="C473" s="7"/>
@@ -27685,7 +27696,7 @@
         <v>889388.28999677394</v>
       </c>
     </row>
-    <row r="475" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F475" s="10"/>
       <c r="G475" s="10"/>
       <c r="H475" s="10"/>
@@ -27699,7 +27710,7 @@
       <c r="P475" s="10"/>
       <c r="Q475" s="10"/>
     </row>
-    <row r="477" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:17" x14ac:dyDescent="0.45">
       <c r="F477" s="10"/>
       <c r="G477" s="10"/>
       <c r="H477" s="10"/>
@@ -27714,6 +27725,18 @@
       <c r="Q477" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:Q473" xr:uid="{3F5400A3-CD7F-49CE-931A-912FD0F3C4E4}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ARAUCA"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="CHIPIRÓN"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
   </mergeCells>
@@ -27864,6 +27887,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -27872,20 +27901,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7A1B6CA-CBCA-491A-A89B-2F3D919BDD3A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7A1B6CA-CBCA-491A-A89B-2F3D919BDD3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4afde810-2293-4670-bb5c-117753097ca5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95E94B4-C040-41BA-90B6-18866C474D53}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13515A21-E437-46BA-A090-A0B1A19BE7F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13515A21-E437-46BA-A090-A0B1A19BE7F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95E94B4-C040-41BA-90B6-18866C474D53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>